<commit_message>
Creacion de modulo apra template xlsx
</commit_message>
<xml_diff>
--- a/src/templates_xlsx/template.xlsx
+++ b/src/templates_xlsx/template.xlsx
@@ -32,11 +32,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -52,6 +53,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -102,12 +110,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -123,24 +135,72 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1882440</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>54000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Imagen 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2700000" cy="729360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3"/>
+  <dimension ref="B3:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.23"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -152,5 +212,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se hace tempaltes de prueba apra pdf y xlsx
</commit_message>
<xml_diff>
--- a/src/templates_xlsx/template.xlsx
+++ b/src/templates_xlsx/template.xlsx
@@ -20,9 +20,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Ejercicio:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:ejercicio}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:Jurisdicción</t>
+  </si>
   <si>
     <t xml:space="preserve">${table:jurisdiccion}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U. Administrativa: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:unidadAdministrativa}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> N° Sucursal: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:sucursal}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° Cuenta:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:nroCuenta}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de Cuenta:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:tipoCuenta}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidad Administrativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° Sucursal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° Cuenta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración Central </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nro. Apertura </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:resumenCuentaCollection.unidadAdministrativaResumen}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:resumenCuentaCollection.sucursalResumen}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:resumenCuentaCollection.nroCuentaResumen}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:resumenCuentaCollection.estadoResumen}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:resumenCuentaCollection.adminCentralResumen}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${table:resumenCuentaCollection.nroAperturaResumen}</t>
   </si>
 </sst>
 </file>
@@ -32,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -62,18 +131,32 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,7 +193,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -121,6 +204,22 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -146,9 +245,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1882440</xdr:colOff>
+      <xdr:colOff>324720</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -162,7 +261,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2700000" cy="729360"/>
+          <a:ext cx="2700000" cy="727920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -182,15 +281,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:B6"/>
+  <dimension ref="A3:F13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.11"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -198,10 +301,92 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
+      <c r="C4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="s">
-        <v>0</v>
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>